<commit_message>
need to see why decomp not working
</commit_message>
<xml_diff>
--- a/output/out_2023-10-30T14:19:55.787/params/params_combined.xlsx
+++ b/output/out_2023-10-30T14:19:55.787/params/params_combined.xlsx
@@ -420,41 +420,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>55</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.15936780329898584</v>
-      </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
-        <v>0.12646051814124454</v>
-      </c>
-      <c r="F2">
-        <v>1.1</v>
-      </c>
-    </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.15971439969654022</v>
+        <v>0.15936780329898584</v>
       </c>
       <c r="D3">
         <v>0.2</v>
       </c>
       <c r="E3">
-        <v>0.14369609644244344</v>
+        <v>0.12646051814124454</v>
       </c>
       <c r="F3">
         <v>1.1</v>
@@ -462,19 +442,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.2722435727399064</v>
+        <v>0.15971439969654022</v>
       </c>
       <c r="D4">
         <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0.2065925884241569</v>
+        <v>0.14369609644244344</v>
       </c>
       <c r="F4">
         <v>1.1</v>
@@ -482,19 +462,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0.1458680148894179</v>
+        <v>0.2722435727399064</v>
       </c>
       <c r="D5">
         <v>0.2</v>
       </c>
       <c r="E5">
-        <v>0.13818979618069932</v>
+        <v>0.2065925884241569</v>
       </c>
       <c r="F5">
         <v>1.1</v>
@@ -502,19 +482,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.15936780329898584</v>
+        <v>0.1458680148894179</v>
       </c>
       <c r="D6">
         <v>0.2</v>
       </c>
       <c r="E6">
-        <v>0.12646051814124454</v>
+        <v>0.13818979618069932</v>
       </c>
       <c r="F6">
         <v>1.1</v>

</xml_diff>